<commit_message>
Common: Updated default atomizers
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/atomizers.xlsx
+++ b/upgrade/fixtures/atomizers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33CC6B49-8108-4530-9480-45D583CE45D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F519D16-E251-49AE-BBBB-3FBEE3D99A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8250" yWindow="4740" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4185" yWindow="2835" windowWidth="33615" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>tab</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>RTA OG 2021</t>
+  </si>
+  <si>
+    <t>dual</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Extreme 2</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Extreme</t>
   </si>
 </sst>
 </file>
@@ -465,10 +480,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124FA0CC-8DC6-4BC4-980D-0724562E5264}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,76 +492,125 @@
     <col min="2" max="2" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A little imrpovement in atomizer import
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/atomizers.xlsx
+++ b/upgrade/fixtures/atomizers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D064848E-80CD-47E0-BEF0-10B32A4AE2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFA0092-E09B-6F40-949F-528D8E9FB50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="2835" windowWidth="33615" windowHeight="18390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <t>tab</t>
   </si>
@@ -100,13 +100,76 @@
     <t>false</t>
   </si>
   <si>
-    <t>Extreme 2</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
-    <t>Extreme</t>
+    <t>Extreme 2 23mm</t>
+  </si>
+  <si>
+    <t>Extreme 23mm</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>RTA</t>
+  </si>
+  <si>
+    <t>RDA</t>
+  </si>
+  <si>
+    <t>RDTA</t>
+  </si>
+  <si>
+    <t>draw</t>
+  </si>
+  <si>
+    <t>Wotofo</t>
+  </si>
+  <si>
+    <t>Recurve V2 RDA</t>
+  </si>
+  <si>
+    <t>Sirius Mods</t>
+  </si>
+  <si>
+    <t>Vega RDA </t>
+  </si>
+  <si>
+    <t>DL, RDL, MTL</t>
+  </si>
+  <si>
+    <t>Dotmod</t>
+  </si>
+  <si>
+    <t>dotRDA Single Coil 22</t>
+  </si>
+  <si>
+    <t>DL, RDL</t>
+  </si>
+  <si>
+    <t>Hussar Vapes</t>
+  </si>
+  <si>
+    <t>Legacy 2 RDA</t>
+  </si>
+  <si>
+    <t>squonk</t>
+  </si>
+  <si>
+    <t>DL</t>
+  </si>
+  <si>
+    <t>MTL, RDL</t>
+  </si>
+  <si>
+    <t>MTL</t>
+  </si>
+  <si>
+    <t>RDL</t>
+  </si>
+  <si>
+    <t>MTL, DL, RDL</t>
   </si>
 </sst>
 </file>
@@ -161,9 +224,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Nadpis 2" xfId="1" builtinId="17"/>
@@ -451,13 +516,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -480,19 +545,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124FA0CC-8DC6-4BC4-980D-0724562E5264}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -502,8 +569,17 @@
       <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -513,8 +589,17 @@
       <c r="C2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -524,8 +609,17 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -535,8 +629,17 @@
       <c r="C4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -546,8 +649,17 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -557,8 +669,17 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -568,8 +689,17 @@
       <c r="C7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -579,8 +709,17 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -590,19 +729,37 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -610,10 +767,105 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" display="https://www.eliquidshop.cz/vyrobce-wotofo-a1010/" xr:uid="{95711F2D-A183-654B-8976-2D692F237083}"/>
+    <hyperlink ref="A13" r:id="rId2" display="https://www.eliquidshop.cz/vyrobce-sirius-mods-a1532/" xr:uid="{2B82FE2D-D14E-664E-9EC1-5A2159CAF7CF}"/>
+    <hyperlink ref="A14" r:id="rId3" display="https://www.eliquidshop.cz/vyrobce-dotmod-a923/" xr:uid="{1589F009-B8C2-2744-AE06-A51C95875D93}"/>
+    <hyperlink ref="A15" r:id="rId4" display="https://www.eliquidshop.cz/vyrobce-hussar-vapes-a1112/" xr:uid="{5D288023-B1E0-C641-AC27-21638FE2A1CC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>